<commit_message>
load characters and dimensions
</commit_message>
<xml_diff>
--- a/Hidden/Assets/Levels/map_schema.xlsx
+++ b/Hidden/Assets/Levels/map_schema.xlsx
@@ -16,20 +16,23 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="map_schema" type="4" refreshedVersion="0" background="1">
+  <connection id="1" name="map" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="D:\U3D\0.PROJECTS\Hidden\Hidden\Hidden\Assets\Levels\map.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="2" name="map_schema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\ljr\Desktop\map_schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" name="map_schema1" type="4" refreshedVersion="0" background="1">
+  <connection id="3" name="map_schema1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\ljr\Desktop\map_schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" name="map_schema2" type="4" refreshedVersion="0" background="1">
+  <connection id="4" name="map_schema2" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\ljr\Desktop\map_schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -74,6 +77,10 @@
     <t>dims.y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>level1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -115,9 +122,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -141,12 +149,12 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema3">
+  <Schema ID="Schema2">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="SavableLevel">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="sLevelName" form="unqualified"/>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:double" name="sLevelName" form="unqualified"/>
             <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="iLevelType" form="unqualified"/>
             <xsd:element minOccurs="0" nillable="true" name="vChar1StartPos" form="unqualified">
               <xsd:complexType>
@@ -157,6 +165,14 @@
               </xsd:complexType>
             </xsd:element>
             <xsd:element minOccurs="0" nillable="true" name="vChar2StartPos" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="x" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="y" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+            <xsd:element minOccurs="0" nillable="true" name="vDim" form="unqualified">
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="x" form="unqualified"/>
@@ -190,27 +206,27 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="3" Name="SavableLevel_映射" RootElement="SavableLevel" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
+  <Map ID="4" Name="SavableLevel_映射" RootElement="SavableLevel" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表4" displayName="表4" ref="A1:C401" tableType="xml" totalsRowShown="0" connectionId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表4" displayName="表4" ref="A1:C401" tableType="xml" totalsRowShown="0" connectionId="1">
   <autoFilter ref="A1:C401"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="x" name="x">
       <calculatedColumnFormula>INT((ROW()-2)/20)</calculatedColumnFormula>
-      <xmlColumnPr mapId="3" xpath="/SavableLevel/tMap/Tile/vTilePosition/x" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/SavableLevel/tMap/Tile/vTilePosition/x" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="y" name="y">
       <calculatedColumnFormula>MOD(ROW()-2,20)</calculatedColumnFormula>
-      <xmlColumnPr mapId="3" xpath="/SavableLevel/tMap/Tile/vTilePosition/y" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/SavableLevel/tMap/Tile/vTilePosition/y" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="iTileType" name="iTileType" dataDxfId="0">
       <calculatedColumnFormula>INDEX('map source data'!$A$1:$T$20,'exportable data'!B2+1,'exportable data'!A2+1)</calculatedColumnFormula>
-      <xmlColumnPr mapId="3" xpath="/SavableLevel/tMap/Tile/iTileType" xmlDataType="integer"/>
+      <xmlColumnPr mapId="4" xpath="/SavableLevel/tMap/Tile/iTileType" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -219,34 +235,44 @@
 
 <file path=xl/tables/tableSingleCells1.xml><?xml version="1.0" encoding="utf-8"?>
 <singleXmlCells xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <singleXmlCell id="8" r="E2" connectionId="3">
-    <xmlCellPr id="1" uniqueName="sLevelName">
-      <xmlPr mapId="3" xpath="/SavableLevel/sLevelName" xmlDataType="string"/>
+  <singleXmlCell id="2" r="F2" connectionId="1">
+    <xmlCellPr id="1" uniqueName="iLevelType">
+      <xmlPr mapId="4" xpath="/SavableLevel/iLevelType" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="9" r="F2" connectionId="3">
-    <xmlCellPr id="1" uniqueName="iLevelType">
-      <xmlPr mapId="3" xpath="/SavableLevel/iLevelType" xmlDataType="integer"/>
+  <singleXmlCell id="3" r="E2" connectionId="1">
+    <xmlCellPr id="1" uniqueName="sLevelName">
+      <xmlPr mapId="4" xpath="/SavableLevel/sLevelName" xmlDataType="double"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="10" r="G2" connectionId="3">
+  <singleXmlCell id="5" r="G2" connectionId="1">
     <xmlCellPr id="1" uniqueName="x">
-      <xmlPr mapId="3" xpath="/SavableLevel/vChar1StartPos/x" xmlDataType="integer"/>
+      <xmlPr mapId="4" xpath="/SavableLevel/vChar1StartPos/x" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="11" r="H2" connectionId="3">
+  <singleXmlCell id="6" r="H2" connectionId="1">
     <xmlCellPr id="1" uniqueName="y">
-      <xmlPr mapId="3" xpath="/SavableLevel/vChar1StartPos/y" xmlDataType="integer"/>
+      <xmlPr mapId="4" xpath="/SavableLevel/vChar1StartPos/y" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="12" r="I2" connectionId="3">
+  <singleXmlCell id="7" r="I2" connectionId="1">
     <xmlCellPr id="1" uniqueName="x">
-      <xmlPr mapId="3" xpath="/SavableLevel/vChar2StartPos/x" xmlDataType="integer"/>
+      <xmlPr mapId="4" xpath="/SavableLevel/vChar2StartPos/x" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="13" r="J2" connectionId="3">
+  <singleXmlCell id="8" r="J2" connectionId="1">
     <xmlCellPr id="1" uniqueName="y">
-      <xmlPr mapId="3" xpath="/SavableLevel/vChar2StartPos/y" xmlDataType="integer"/>
+      <xmlPr mapId="4" xpath="/SavableLevel/vChar2StartPos/y" xmlDataType="integer"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="9" r="K2" connectionId="1">
+    <xmlCellPr id="1" uniqueName="x">
+      <xmlPr mapId="4" xpath="/SavableLevel/vDim/x" xmlDataType="integer"/>
+    </xmlCellPr>
+  </singleXmlCell>
+  <singleXmlCell id="10" r="L2" connectionId="1">
+    <xmlCellPr id="1" uniqueName="y">
+      <xmlPr mapId="4" xpath="/SavableLevel/vDim/y" xmlDataType="integer"/>
     </xmlCellPr>
   </singleXmlCell>
 </singleXmlCells>
@@ -1007,21 +1033,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M401"/>
+  <dimension ref="A1:L401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="4.75" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="4.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="7.5" customWidth="1"/>
+    <col min="7" max="12" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1049,14 +1075,14 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
       <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2">
         <f>INT((ROW()-2)/20)</f>
         <v>0</v>
@@ -1069,8 +1095,8 @@
         <f>INDEX('map source data'!$A$1:$T$20,'exportable data'!B2+1,'exportable data'!A2+1)</f>
         <v>2</v>
       </c>
-      <c r="E2" s="1">
-        <v>1.1000000000000001</v>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1086,15 +1112,15 @@
       </c>
       <c r="J2">
         <v>2</v>
+      </c>
+      <c r="K2">
+        <v>20</v>
       </c>
       <c r="L2">
         <v>20</v>
       </c>
-      <c r="M2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">INT((ROW()-2)/20)</f>
         <v>0</v>
@@ -1108,7 +1134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1122,7 +1148,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1136,7 +1162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1150,7 +1176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1164,7 +1190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1178,7 +1204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1192,7 +1218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1206,7 +1232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1220,7 +1246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1234,7 +1260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1248,7 +1274,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1262,7 +1288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1276,7 +1302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6472,11 +6498,11 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A387">
-        <f t="shared" ref="A387:A450" si="12">INT((ROW()-2)/20)</f>
+        <f t="shared" ref="A387:A401" si="12">INT((ROW()-2)/20)</f>
         <v>19</v>
       </c>
       <c r="B387">
-        <f t="shared" ref="B387:B450" si="13">MOD(ROW()-2,20)</f>
+        <f t="shared" ref="B387:B401" si="13">MOD(ROW()-2,20)</f>
         <v>5</v>
       </c>
       <c r="C387">

</xml_diff>